<commit_message>
Diverse småoppdateringer i ekstra
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-H21.xlsx
+++ b/diverse/tidsplan-H21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s14363\Documents\temp2\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1941412-0A63-4ACD-8C36-184DCB94B6C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BD6405-A96C-4146-AE25-2BEDE1B1B8FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Uke</t>
   </si>
@@ -75,82 +75,79 @@
     <t>Regresjon og Dataøving 2</t>
   </si>
   <si>
-    <t>Ingen aktivitet</t>
-  </si>
-  <si>
-    <t>26.08: Introduksjon til R i Aud Max</t>
-  </si>
-  <si>
-    <t>30.08: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom</t>
-  </si>
-  <si>
     <t>02.09: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
   </si>
   <si>
-    <t>13.09: Kontakttime, kkursansvarlig tilgjengelig i Aud A/zoom</t>
-  </si>
-  <si>
     <t>16.09: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
   </si>
   <si>
-    <t>20.09: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom</t>
-  </si>
-  <si>
-    <t>23.09: Kontakttime, kursansvarlig tilgjengelig på Aud Max/Zoom</t>
-  </si>
-  <si>
     <t>30.09: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
   </si>
   <si>
-    <t>04.10: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom</t>
-  </si>
-  <si>
     <t>07.10: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
   </si>
   <si>
-    <t>11.10: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom</t>
-  </si>
-  <si>
-    <t>18.10: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom</t>
-  </si>
-  <si>
     <t>21.10: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
   </si>
   <si>
-    <t>25.10: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom</t>
-  </si>
-  <si>
-    <t>1.11: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom</t>
-  </si>
-  <si>
     <t>Forberedelse/HEKS</t>
   </si>
   <si>
     <t>Forberedelse/IEKS</t>
   </si>
   <si>
-    <t>08.11: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom</t>
-  </si>
-  <si>
     <t>11.11 Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
   </si>
   <si>
-    <t>Karrieredager NHH - ingen forelesninger</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>4.11: **Oversiktsforelesning: Tidsrekker** i Aud Max</t>
-  </si>
-  <si>
-    <t>28.10: **Oversiktsforelesning: Regresjon** i Aud Max</t>
-  </si>
-  <si>
-    <t>14.10: **Oversiktsforelesning: Hypotesetesting** i Aud Max</t>
-  </si>
-  <si>
-    <t>23.08: Intro om Met4 og kursopplegget i år</t>
+    <t>23.08: Intro om Met4 og kursopplegget i år.</t>
+  </si>
+  <si>
+    <t>30.08: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom.</t>
+  </si>
+  <si>
+    <t>Karrieredager NHH - ingen forelesninger.</t>
+  </si>
+  <si>
+    <t>13.09: Kontakttime, kkursansvarlig tilgjengelig i Aud A/zoom.</t>
+  </si>
+  <si>
+    <t>20.09: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom.</t>
+  </si>
+  <si>
+    <t>Ingen aktivitet.</t>
+  </si>
+  <si>
+    <t>04.10: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom.</t>
+  </si>
+  <si>
+    <t>11.10: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom.</t>
+  </si>
+  <si>
+    <t>18.10: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom.</t>
+  </si>
+  <si>
+    <t>25.10: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom.</t>
+  </si>
+  <si>
+    <t>1.11: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom.</t>
+  </si>
+  <si>
+    <t>08.11: Kontakttime, kursansvarlig tilgjengelig i Aud A/zoom.</t>
+  </si>
+  <si>
+    <t>26.08: Introduksjon til R i Aud Max.</t>
+  </si>
+  <si>
+    <t>23.09: Kontakttime, kursansvarlig tilgjengelig på Aud Max/Zoom.</t>
+  </si>
+  <si>
+    <t>14.10: **Oversiktsforelesning: Hypotesetesting** i Aud Max.</t>
+  </si>
+  <si>
+    <t>28.10: **Oversiktsforelesning: Regresjon** i Aud Max.</t>
+  </si>
+  <si>
+    <t>4.11: **Oversiktsforelesning: Tidsrekker** i Aud Max.</t>
   </si>
 </sst>
 </file>
@@ -172,18 +169,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -198,11 +189,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,17 +471,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="4" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="124.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -519,10 +508,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -533,10 +522,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -546,10 +535,9 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="1"/>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -559,10 +547,10 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -573,10 +561,10 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,10 +575,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -601,10 +589,10 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -615,10 +603,10 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -629,10 +617,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -643,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>39</v>
@@ -657,10 +645,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -671,10 +659,10 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,7 +670,7 @@
         <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -690,19 +678,12 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C4:D4"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Nye oppgaver og div info
</commit_message>
<xml_diff>
--- a/diverse/tidsplan-H21.xlsx
+++ b/diverse/tidsplan-H21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s14363\Documents\temp2\met4\diverse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C971D638-D632-44EB-AFA1-FFC735301F2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869AA8AA-8C73-4B59-9F73-0ED52BD42438}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,24 +75,9 @@
     <t>Regresjon og Dataøving 2</t>
   </si>
   <si>
-    <t>02.09: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
-    <t>16.09: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
-    <t>30.09: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
     <t>07.10: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
   </si>
   <si>
-    <t>21.10: Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
-    <t>11.11 Oppgaveseminar Aud Max. Se \@ref(seminar) for oppgaver.</t>
-  </si>
-  <si>
     <t>23.08: Intro om Met4 og kursopplegget i år.</t>
   </si>
   <si>
@@ -105,15 +90,6 @@
     <t>26.08: Introduksjon til R i Aud Max.</t>
   </si>
   <si>
-    <t>14.10: **Oversiktsforelesning: Hypotesetesting** i Aud Max.</t>
-  </si>
-  <si>
-    <t>28.10: **Oversiktsforelesning: Regresjon** i Aud Max.</t>
-  </si>
-  <si>
-    <t>4.11: **Oversiktsforelesning: Tidsrekker** i Aud Max.</t>
-  </si>
-  <si>
     <t>30.08: Kontakttime, kursansvarlig tilgjengelig i Aud A/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 ).</t>
   </si>
   <si>
@@ -142,6 +118,30 @@
   </si>
   <si>
     <t>23.09: Kontakttime, kursansvarlig tilgjengelig på Aud Max/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 ).</t>
+  </si>
+  <si>
+    <t>02.09: Oppgaveseminar Aud Max/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 ).. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>16.09: Oppgaveseminar Aud Max/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 ).. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>30.09: Oppgaveseminar Aud Max/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 ).. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>14.10: **Oversiktsforelesning: Hypotesetesting** i Aud Max/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 )..</t>
+  </si>
+  <si>
+    <t>21.10: Oppgaveseminar Aud Max/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 ).. Se \@ref(seminar) for oppgaver.</t>
+  </si>
+  <si>
+    <t>28.10: **Oversiktsforelesning: Regresjon** i Aud Max/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 )..</t>
+  </si>
+  <si>
+    <t>4.11: **Oversiktsforelesning: Tidsrekker** i Aud Max/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 )..</t>
+  </si>
+  <si>
+    <t>11.11 Oppgaveseminar Aud Max/[Zoom](https://nhh.zoom.us/j/66295455298?pwd=bWNBd2NlUE9PLzRCNHZQUEVuaVE1UT09 ).. Se \@ref(seminar) for oppgaver.</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,10 +502,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,7 +530,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -541,10 +541,10 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -555,10 +555,10 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -569,10 +569,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,10 +583,10 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -597,10 +597,10 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,10 +611,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,10 +625,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -639,10 +639,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -653,10 +653,10 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>